<commit_message>
AITATR3-219 Revisi no1 & AITATR3-202
</commit_message>
<xml_diff>
--- a/Rule/AssetRegionRule.xlsx
+++ b/Rule/AssetRegionRule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.sucipto\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teresa.octaviani\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19120" windowHeight="7000"/>
   </bookViews>
   <sheets>
     <sheet name="InsRegion" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>DATA OBJECTS</t>
   </si>
@@ -59,21 +59,6 @@
     <t>AppAsset.TaxCityIssuer == @val</t>
   </si>
   <si>
-    <t>Jakarta Barat ., Wil. Kota</t>
-  </si>
-  <si>
-    <t>Bangkalan, Kab.</t>
-  </si>
-  <si>
-    <t>Aceh Barat Daya, Kab.</t>
-  </si>
-  <si>
-    <t>Aceh Jeumpa/Bireuen, Kab.</t>
-  </si>
-  <si>
-    <t>Yogyakarta, Kota.</t>
-  </si>
-  <si>
     <t>AppCollateralRegistration</t>
   </si>
   <si>
@@ -83,9 +68,6 @@
     <t>AppObj.OriginalCityLocation == @val</t>
   </si>
   <si>
-    <t>Tangerang</t>
-  </si>
-  <si>
     <t>AssetRegion</t>
   </si>
   <si>
@@ -101,12 +83,6 @@
     <t>REGION2</t>
   </si>
   <si>
-    <t>Padang Pariaman</t>
-  </si>
-  <si>
-    <t>Padang Pariaman, Kab.</t>
-  </si>
-  <si>
     <t>SETTINGS</t>
   </si>
   <si>
@@ -117,13 +93,58 @@
   </si>
   <si>
     <t>EXIT_WHEN_FOUND</t>
+  </si>
+  <si>
+    <t>JAKARTA BARAT ., WIL. KOTA</t>
+  </si>
+  <si>
+    <t>BANGKALAN, KAB.</t>
+  </si>
+  <si>
+    <t>ACEH BARAT DAYA, KAB.</t>
+  </si>
+  <si>
+    <t>YOGYAKARTA, KOTA.</t>
+  </si>
+  <si>
+    <t>PADANG PARIAMAN, KAB.</t>
+  </si>
+  <si>
+    <t>TANGERANG, KAB.</t>
+  </si>
+  <si>
+    <t>TANGERANG, KOTA.</t>
+  </si>
+  <si>
+    <t>TANGSEL</t>
+  </si>
+  <si>
+    <t>JAKARTA BARAT</t>
+  </si>
+  <si>
+    <t>TANGERANG</t>
+  </si>
+  <si>
+    <t>TANGERANG SELATAN</t>
+  </si>
+  <si>
+    <t>BANGKALAN</t>
+  </si>
+  <si>
+    <t>ACEH BARAT DAYA</t>
+  </si>
+  <si>
+    <t>YOGYAKARTA</t>
+  </si>
+  <si>
+    <t>PADANG PARIAMAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +169,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -194,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -206,6 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,26 +515,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -513,7 +542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -522,16 +551,16 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -540,43 +569,43 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B10" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -584,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -598,138 +627,152 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>